<commit_message>
fix hellwig data in hellwig and summary spreadsheet
</commit_message>
<xml_diff>
--- a/Methods/HELLWIG/Matura2020_ranking_Hellwig.xlsx
+++ b/Methods/HELLWIG/Matura2020_ranking_Hellwig.xlsx
@@ -88,6 +88,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -109,6 +110,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -166,7 +168,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -177,6 +179,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -259,13 +265,13 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:B1"/>
+      <selection pane="topLeft" activeCell="H6" activeCellId="0" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.95"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -280,128 +286,128 @@
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="n">
-        <v>0.8</v>
+      <c r="B2" s="3" t="n">
+        <v>0.243164</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2" t="n">
-        <v>0.67</v>
+      <c r="B3" s="3" t="n">
+        <v>0.246206</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="2" t="n">
-        <v>0.56</v>
+      <c r="B4" s="3" t="n">
+        <v>0.30354</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="2" t="n">
-        <v>0.42</v>
+      <c r="B5" s="3" t="n">
+        <v>0.208139</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="2" t="n">
-        <v>0.41</v>
+      <c r="B6" s="3" t="n">
+        <v>0.339088</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="2" t="n">
-        <v>0.37</v>
+      <c r="B7" s="3" t="n">
+        <v>0.667013</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="2" t="n">
-        <v>0.35</v>
+      <c r="B8" s="3" t="n">
+        <v>0.795715</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="2" t="n">
-        <v>0.34</v>
+      <c r="B9" s="3" t="n">
+        <v>0.140076</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="2" t="n">
-        <v>0.34</v>
+      <c r="B10" s="3" t="n">
+        <v>0.225525</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="2" t="n">
-        <v>0.3</v>
+      <c r="B11" s="3" t="n">
+        <v>0.561972</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="2" t="n">
-        <v>0.25</v>
+      <c r="B12" s="3" t="n">
+        <v>0.408323</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="2" t="n">
-        <v>0.24</v>
+      <c r="B13" s="3" t="n">
+        <v>0.421173</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="2" t="n">
-        <v>0.23</v>
+      <c r="B14" s="3" t="n">
+        <v>0.339127</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="2" t="n">
-        <v>0.21</v>
+      <c r="B15" s="3" t="n">
+        <v>0.112509</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="2" t="n">
-        <v>0.14</v>
+      <c r="B16" s="3" t="n">
+        <v>0.36864</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="2" t="n">
-        <v>0.11</v>
+      <c r="B17" s="3" t="n">
+        <v>0.3473</v>
       </c>
     </row>
   </sheetData>

</xml_diff>